<commit_message>
Update Backlog Dries Claesen .xlsx
</commit_message>
<xml_diff>
--- a/PV/Backlog Dries Claesen .xlsx
+++ b/PV/Backlog Dries Claesen .xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93b1d1b505b883ae/Documenten/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3scla\OneDrive\Documenten\GitHub\pv-1819-dries.claesen\PV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA79C79C-606E-418B-8106-5924A3A65785}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{FA79C79C-606E-418B-8106-5924A3A65785}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{5E6E62FA-2A46-4BA2-88DC-7E7969F056DE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -780,43 +780,43 @@
                   <c:v>5.5714285714285712</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.1428571428571423</c:v>
+                  <c:v>5.4285714285714279</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.7142857142857135</c:v>
+                  <c:v>5.2857142857142847</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.2857142857142847</c:v>
+                  <c:v>5.1428571428571415</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.8571428571428563</c:v>
+                  <c:v>4.9999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.4285714285714279</c:v>
+                  <c:v>4.857142857142855</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.9999999999999996</c:v>
+                  <c:v>4.7142857142857117</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5714285714285712</c:v>
+                  <c:v>4.5714285714285685</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.1428571428571428</c:v>
+                  <c:v>4.4285714285714253</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.7142857142857142</c:v>
+                  <c:v>4.285714285714282</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.2857142857142856</c:v>
+                  <c:v>4.1428571428571388</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.85714285714285698</c:v>
+                  <c:v>3.999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.42857142857142844</c:v>
+                  <c:v>3.8571428571428532</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>3.7142857142857104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -912,46 +912,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2274,7 +2274,7 @@
   <dimension ref="A1:IV17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15" customHeight="1"/>
@@ -2397,7 +2397,9 @@
       <c r="D4" s="11">
         <v>2</v>
       </c>
-      <c r="E4" s="11"/>
+      <c r="E4" s="11">
+        <v>4</v>
+      </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -2624,59 +2626,59 @@
       </c>
       <c r="E12" s="14">
         <f t="shared" ref="E12:R12" si="0">D12-SUM(E4:E11)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F12" s="14">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G12" s="14">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H12" s="14">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I12" s="14">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J12" s="14">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K12" s="14">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L12" s="14">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M12" s="14">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="N12" s="14">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="O12" s="14">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="P12" s="14">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="Q12" s="14">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="R12" s="14">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="S12" s="15"/>
       <c r="T12" s="15"/>
@@ -2768,55 +2770,55 @@
       </c>
       <c r="AC16" s="22">
         <f t="shared" si="1"/>
-        <v>5.1428571428571423</v>
+        <v>5.4285714285714279</v>
       </c>
       <c r="AD16" s="22">
         <f t="shared" si="1"/>
-        <v>4.7142857142857135</v>
+        <v>5.2857142857142847</v>
       </c>
       <c r="AE16" s="22">
         <f t="shared" si="1"/>
-        <v>4.2857142857142847</v>
+        <v>5.1428571428571415</v>
       </c>
       <c r="AF16" s="22">
         <f t="shared" si="1"/>
-        <v>3.8571428571428563</v>
+        <v>4.9999999999999982</v>
       </c>
       <c r="AG16" s="22">
         <f t="shared" si="1"/>
-        <v>3.4285714285714279</v>
+        <v>4.857142857142855</v>
       </c>
       <c r="AH16" s="22">
         <f t="shared" si="1"/>
-        <v>2.9999999999999996</v>
+        <v>4.7142857142857117</v>
       </c>
       <c r="AI16" s="22">
         <f t="shared" si="1"/>
-        <v>2.5714285714285712</v>
+        <v>4.5714285714285685</v>
       </c>
       <c r="AJ16" s="22">
         <f t="shared" si="1"/>
-        <v>2.1428571428571428</v>
+        <v>4.4285714285714253</v>
       </c>
       <c r="AK16" s="22">
         <f t="shared" si="1"/>
-        <v>1.7142857142857142</v>
+        <v>4.285714285714282</v>
       </c>
       <c r="AL16" s="22">
         <f t="shared" si="1"/>
-        <v>1.2857142857142856</v>
+        <v>4.1428571428571388</v>
       </c>
       <c r="AM16" s="22">
         <f t="shared" si="1"/>
-        <v>0.85714285714285698</v>
+        <v>3.999999999999996</v>
       </c>
       <c r="AN16" s="22">
         <f t="shared" si="1"/>
-        <v>0.42857142857142844</v>
+        <v>3.8571428571428532</v>
       </c>
       <c r="AO16" s="23">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.7142857142857104</v>
       </c>
     </row>
     <row r="17" spans="26:41" ht="20.7" customHeight="1">
@@ -2829,59 +2831,59 @@
       </c>
       <c r="AB17" s="25">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AC17" s="25">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AD17" s="25">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AE17" s="25">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AF17" s="25">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AG17" s="25">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AH17" s="25">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AI17" s="25">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AJ17" s="25">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AK17" s="25">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AL17" s="25">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AM17" s="25">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AN17" s="25">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AO17" s="26">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>